<commit_message>
Problem 2 calibration and demand prediction added
</commit_message>
<xml_diff>
--- a/Distances.xlsx
+++ b/Distances.xlsx
@@ -340,13 +340,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T20"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:24">
       <c r="A1">
         <v>0</v>
       </c>
@@ -407,8 +407,20 @@
       <c r="T1">
         <v>2472</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="U1">
+        <v>5541</v>
+      </c>
+      <c r="V1">
+        <v>7764</v>
+      </c>
+      <c r="W1">
+        <v>8762</v>
+      </c>
+      <c r="X1">
+        <v>6345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2">
         <v>347</v>
       </c>
@@ -469,8 +481,20 @@
       <c r="T2">
         <v>2422</v>
       </c>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="U2">
+        <v>5835</v>
+      </c>
+      <c r="V2">
+        <v>8073</v>
+      </c>
+      <c r="W2">
+        <v>9105</v>
+      </c>
+      <c r="X2">
+        <v>6666</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3">
         <v>370</v>
       </c>
@@ -531,8 +555,20 @@
       <c r="T3">
         <v>2784</v>
       </c>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="U3">
+        <v>5849</v>
+      </c>
+      <c r="V3">
+        <v>8051</v>
+      </c>
+      <c r="W3">
+        <v>8958</v>
+      </c>
+      <c r="X3">
+        <v>6613</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4">
         <v>654</v>
       </c>
@@ -593,8 +629,20 @@
       <c r="T4">
         <v>2836</v>
       </c>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="U4">
+        <v>6191</v>
+      </c>
+      <c r="V4">
+        <v>8404</v>
+      </c>
+      <c r="W4">
+        <v>9324</v>
+      </c>
+      <c r="X4">
+        <v>6973</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5">
         <v>1246</v>
       </c>
@@ -655,8 +703,20 @@
       <c r="T5">
         <v>1460</v>
       </c>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="U5">
+        <v>5763</v>
+      </c>
+      <c r="V5">
+        <v>8041</v>
+      </c>
+      <c r="W5">
+        <v>9389</v>
+      </c>
+      <c r="X5">
+        <v>6747</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6">
         <v>1148</v>
       </c>
@@ -717,8 +777,20 @@
       <c r="T6">
         <v>1922</v>
       </c>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="U6">
+        <v>6152</v>
+      </c>
+      <c r="V6">
+        <v>8427</v>
+      </c>
+      <c r="W6">
+        <v>9677</v>
+      </c>
+      <c r="X6">
+        <v>7095</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7">
         <v>941</v>
       </c>
@@ -779,8 +851,20 @@
       <c r="T7">
         <v>2948</v>
       </c>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="U7">
+        <v>6483</v>
+      </c>
+      <c r="V7">
+        <v>8700</v>
+      </c>
+      <c r="W7">
+        <v>9618</v>
+      </c>
+      <c r="X7">
+        <v>7271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8">
         <v>1444</v>
       </c>
@@ -841,8 +925,20 @@
       <c r="T8">
         <v>2744</v>
       </c>
-    </row>
-    <row r="9" spans="1:20">
+      <c r="U8">
+        <v>6867</v>
+      </c>
+      <c r="V8">
+        <v>9127</v>
+      </c>
+      <c r="W8">
+        <v>10206</v>
+      </c>
+      <c r="X8">
+        <v>7744</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9">
         <v>449</v>
       </c>
@@ -903,8 +999,20 @@
       <c r="T9">
         <v>2451</v>
       </c>
-    </row>
-    <row r="10" spans="1:20">
+      <c r="U9">
+        <v>5104</v>
+      </c>
+      <c r="V9">
+        <v>7319</v>
+      </c>
+      <c r="W9">
+        <v>8320</v>
+      </c>
+      <c r="X9">
+        <v>5897</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10">
         <v>1462</v>
       </c>
@@ -965,8 +1073,20 @@
       <c r="T10">
         <v>3930</v>
       </c>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="U10">
+        <v>6293</v>
+      </c>
+      <c r="V10">
+        <v>8343</v>
+      </c>
+      <c r="W10">
+        <v>8865</v>
+      </c>
+      <c r="X10">
+        <v>6857</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11">
         <v>1564</v>
       </c>
@@ -1027,8 +1147,20 @@
       <c r="T11">
         <v>965</v>
       </c>
-    </row>
-    <row r="12" spans="1:20">
+      <c r="U11">
+        <v>5406</v>
+      </c>
+      <c r="V11">
+        <v>7678</v>
+      </c>
+      <c r="W11">
+        <v>9139</v>
+      </c>
+      <c r="X11">
+        <v>6437</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
       <c r="A12">
         <v>947</v>
       </c>
@@ -1089,8 +1221,20 @@
       <c r="T12">
         <v>3263</v>
       </c>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="U12">
+        <v>6369</v>
+      </c>
+      <c r="V12">
+        <v>8540</v>
+      </c>
+      <c r="W12">
+        <v>9321</v>
+      </c>
+      <c r="X12">
+        <v>7083</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
       <c r="A13">
         <v>1848</v>
       </c>
@@ -1151,8 +1295,20 @@
       <c r="T13">
         <v>4306</v>
       </c>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="U13">
+        <v>6609</v>
+      </c>
+      <c r="V13">
+        <v>8610</v>
+      </c>
+      <c r="W13">
+        <v>9016</v>
+      </c>
+      <c r="X13">
+        <v>7121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
       <c r="A14">
         <v>1470</v>
       </c>
@@ -1213,8 +1369,20 @@
       <c r="T14">
         <v>3715</v>
       </c>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="U14">
+        <v>6849</v>
+      </c>
+      <c r="V14">
+        <v>8990</v>
+      </c>
+      <c r="W14">
+        <v>9661</v>
+      </c>
+      <c r="X14">
+        <v>7521</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
       <c r="A15">
         <v>533</v>
       </c>
@@ -1275,8 +1443,20 @@
       <c r="T15">
         <v>2786</v>
       </c>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="U15">
+        <v>5226</v>
+      </c>
+      <c r="V15">
+        <v>7405</v>
+      </c>
+      <c r="W15">
+        <v>8294</v>
+      </c>
+      <c r="X15">
+        <v>5958</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
       <c r="A16">
         <v>2104</v>
       </c>
@@ -1337,8 +1517,20 @@
       <c r="T16">
         <v>3899</v>
       </c>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="U16">
+        <v>7633</v>
+      </c>
+      <c r="V16">
+        <v>9825</v>
+      </c>
+      <c r="W16">
+        <v>10580</v>
+      </c>
+      <c r="X16">
+        <v>8373</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
       <c r="A17">
         <v>2715</v>
       </c>
@@ -1399,8 +1591,20 @@
       <c r="T17">
         <v>3850</v>
       </c>
-    </row>
-    <row r="18" spans="1:20">
+      <c r="U17">
+        <v>8199</v>
+      </c>
+      <c r="V17">
+        <v>10454</v>
+      </c>
+      <c r="W17">
+        <v>11435</v>
+      </c>
+      <c r="X17">
+        <v>9056</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24">
       <c r="A18">
         <v>1895</v>
       </c>
@@ -1461,8 +1665,20 @@
       <c r="T18">
         <v>3503</v>
       </c>
-    </row>
-    <row r="19" spans="1:20">
+      <c r="U18">
+        <v>4164</v>
+      </c>
+      <c r="V18">
+        <v>6207</v>
+      </c>
+      <c r="W18">
+        <v>6928</v>
+      </c>
+      <c r="X18">
+        <v>4726</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24">
       <c r="A19">
         <v>1834</v>
       </c>
@@ -1523,8 +1739,20 @@
       <c r="T19">
         <v>2780</v>
       </c>
-    </row>
-    <row r="20" spans="1:20">
+      <c r="U19">
+        <v>7161</v>
+      </c>
+      <c r="V19">
+        <v>9432</v>
+      </c>
+      <c r="W19">
+        <v>10583</v>
+      </c>
+      <c r="X19">
+        <v>8075</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
       <c r="A20">
         <v>2472</v>
       </c>
@@ -1583,6 +1811,314 @@
         <v>2780</v>
       </c>
       <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>5072</v>
+      </c>
+      <c r="V20">
+        <v>7286</v>
+      </c>
+      <c r="W20">
+        <v>8981</v>
+      </c>
+      <c r="X20">
+        <v>6194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24">
+      <c r="A21">
+        <v>5541</v>
+      </c>
+      <c r="B21">
+        <v>5835</v>
+      </c>
+      <c r="C21">
+        <v>5849</v>
+      </c>
+      <c r="D21">
+        <v>6191</v>
+      </c>
+      <c r="E21">
+        <v>5763</v>
+      </c>
+      <c r="F21">
+        <v>6152</v>
+      </c>
+      <c r="G21">
+        <v>6483</v>
+      </c>
+      <c r="H21">
+        <v>6867</v>
+      </c>
+      <c r="I21">
+        <v>5104</v>
+      </c>
+      <c r="J21">
+        <v>6293</v>
+      </c>
+      <c r="K21">
+        <v>5406</v>
+      </c>
+      <c r="L21">
+        <v>6369</v>
+      </c>
+      <c r="M21">
+        <v>6609</v>
+      </c>
+      <c r="N21">
+        <v>6849</v>
+      </c>
+      <c r="O21">
+        <v>5226</v>
+      </c>
+      <c r="P21">
+        <v>7633</v>
+      </c>
+      <c r="Q21">
+        <v>8199</v>
+      </c>
+      <c r="R21">
+        <v>4164</v>
+      </c>
+      <c r="S21">
+        <v>7161</v>
+      </c>
+      <c r="T21">
+        <v>5072</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>2277</v>
+      </c>
+      <c r="W21">
+        <v>3975</v>
+      </c>
+      <c r="X21">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24">
+      <c r="A22">
+        <v>7764</v>
+      </c>
+      <c r="B22">
+        <v>8073</v>
+      </c>
+      <c r="C22">
+        <v>8051</v>
+      </c>
+      <c r="D22">
+        <v>8404</v>
+      </c>
+      <c r="E22">
+        <v>8041</v>
+      </c>
+      <c r="F22">
+        <v>8427</v>
+      </c>
+      <c r="G22">
+        <v>8700</v>
+      </c>
+      <c r="H22">
+        <v>9127</v>
+      </c>
+      <c r="I22">
+        <v>7319</v>
+      </c>
+      <c r="J22">
+        <v>8343</v>
+      </c>
+      <c r="K22">
+        <v>7678</v>
+      </c>
+      <c r="L22">
+        <v>8540</v>
+      </c>
+      <c r="M22">
+        <v>8610</v>
+      </c>
+      <c r="N22">
+        <v>8990</v>
+      </c>
+      <c r="O22">
+        <v>7405</v>
+      </c>
+      <c r="P22">
+        <v>9825</v>
+      </c>
+      <c r="Q22">
+        <v>10454</v>
+      </c>
+      <c r="R22">
+        <v>6207</v>
+      </c>
+      <c r="S22">
+        <v>9432</v>
+      </c>
+      <c r="T22">
+        <v>7286</v>
+      </c>
+      <c r="U22">
+        <v>2277</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>2216</v>
+      </c>
+      <c r="X22">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24">
+      <c r="A23">
+        <v>8762</v>
+      </c>
+      <c r="B23">
+        <v>9105</v>
+      </c>
+      <c r="C23">
+        <v>8958</v>
+      </c>
+      <c r="D23">
+        <v>9324</v>
+      </c>
+      <c r="E23">
+        <v>9389</v>
+      </c>
+      <c r="F23">
+        <v>9677</v>
+      </c>
+      <c r="G23">
+        <v>9618</v>
+      </c>
+      <c r="H23">
+        <v>10206</v>
+      </c>
+      <c r="I23">
+        <v>8320</v>
+      </c>
+      <c r="J23">
+        <v>8865</v>
+      </c>
+      <c r="K23">
+        <v>9139</v>
+      </c>
+      <c r="L23">
+        <v>9321</v>
+      </c>
+      <c r="M23">
+        <v>9016</v>
+      </c>
+      <c r="N23">
+        <v>9661</v>
+      </c>
+      <c r="O23">
+        <v>8294</v>
+      </c>
+      <c r="P23">
+        <v>10580</v>
+      </c>
+      <c r="Q23">
+        <v>11435</v>
+      </c>
+      <c r="R23">
+        <v>6928</v>
+      </c>
+      <c r="S23">
+        <v>10583</v>
+      </c>
+      <c r="T23">
+        <v>8981</v>
+      </c>
+      <c r="U23">
+        <v>3975</v>
+      </c>
+      <c r="V23">
+        <v>2216</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>2802</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24">
+      <c r="A24">
+        <v>6345</v>
+      </c>
+      <c r="B24">
+        <v>6666</v>
+      </c>
+      <c r="C24">
+        <v>6613</v>
+      </c>
+      <c r="D24">
+        <v>6973</v>
+      </c>
+      <c r="E24">
+        <v>6747</v>
+      </c>
+      <c r="F24">
+        <v>7095</v>
+      </c>
+      <c r="G24">
+        <v>7271</v>
+      </c>
+      <c r="H24">
+        <v>7744</v>
+      </c>
+      <c r="I24">
+        <v>5897</v>
+      </c>
+      <c r="J24">
+        <v>6857</v>
+      </c>
+      <c r="K24">
+        <v>6437</v>
+      </c>
+      <c r="L24">
+        <v>7083</v>
+      </c>
+      <c r="M24">
+        <v>7121</v>
+      </c>
+      <c r="N24">
+        <v>7521</v>
+      </c>
+      <c r="O24">
+        <v>5958</v>
+      </c>
+      <c r="P24">
+        <v>8373</v>
+      </c>
+      <c r="Q24">
+        <v>9056</v>
+      </c>
+      <c r="R24">
+        <v>4726</v>
+      </c>
+      <c r="S24">
+        <v>8075</v>
+      </c>
+      <c r="T24">
+        <v>6194</v>
+      </c>
+      <c r="U24">
+        <v>1188</v>
+      </c>
+      <c r="V24">
+        <v>1490</v>
+      </c>
+      <c r="W24">
+        <v>2802</v>
+      </c>
+      <c r="X24">
         <v>0</v>
       </c>
     </row>

</xml_diff>